<commit_message>
Added all data from excel to our suggestion engine.
- Changed dose from double to string
- Created a python script to read excel files and spit out required code
  in Dart for our suggestion engine
</commit_message>
<xml_diff>
--- a/pesticides/croatia/Maize and wheat.xlsx
+++ b/pesticides/croatia/Maize and wheat.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940730D1-CF4F-1245-828C-9B2B28342B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4590" activeTab="6"/>
+    <workbookView xWindow="-32420" yWindow="13420" windowWidth="32420" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sunn pest" sheetId="1" r:id="rId1"/>
@@ -21,16 +22,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -470,9 +461,6 @@
     <t xml:space="preserve">      Ostrinia nubilalis</t>
   </si>
   <si>
-    <t>Eur. corn borer</t>
-  </si>
-  <si>
     <t>25g/ l Deltametrin</t>
   </si>
   <si>
@@ -573,12 +561,15 @@
   </si>
   <si>
     <t>W.corn rootw. Kuk.zlatica</t>
+  </si>
+  <si>
+    <t>European corn borer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -735,85 +726,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1083,35 +1072,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="6" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="6" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1122,23 +1111,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1148,22 +1137,22 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>137</v>
@@ -1172,18 +1161,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>135</v>
@@ -1192,67 +1181,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F6" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F7" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="F8" s="4">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1260,185 +1249,185 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" t="s">
         <v>161</v>
-      </c>
-      <c r="E14" t="s">
-        <v>162</v>
       </c>
       <c r="F14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="B15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15" t="s">
-        <v>158</v>
-      </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="E15" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F15">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F16">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" t="s">
         <v>157</v>
       </c>
-      <c r="B17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" t="s">
-        <v>158</v>
-      </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F17">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="F18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B19" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" t="s">
-        <v>158</v>
-      </c>
-      <c r="D19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19" t="s">
-        <v>172</v>
-      </c>
-      <c r="F19">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F20">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" t="s">
         <v>157</v>
       </c>
-      <c r="B21" t="s">
-        <v>167</v>
-      </c>
-      <c r="C21" t="s">
-        <v>158</v>
-      </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E21" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F21">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>156</v>
+      </c>
+      <c r="B22" t="s">
+        <v>166</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F38">
     <sortCondition ref="D1"/>
   </sortState>
   <mergeCells count="5">
@@ -1454,29 +1443,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1487,23 +1476,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1513,11 +1502,11 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1537,7 +1526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1557,7 +1546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -1568,9 +1557,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
         <v>140</v>
@@ -1588,9 +1577,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
         <v>140</v>
@@ -1599,18 +1588,18 @@
         <v>143</v>
       </c>
       <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" t="s">
         <v>145</v>
-      </c>
-      <c r="E12" t="s">
-        <v>146</v>
       </c>
       <c r="F12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
         <v>140</v>
@@ -1619,18 +1608,18 @@
         <v>143</v>
       </c>
       <c r="D13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" t="s">
         <v>147</v>
-      </c>
-      <c r="E13" t="s">
-        <v>148</v>
       </c>
       <c r="F13">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s">
         <v>140</v>
@@ -1639,7 +1628,7 @@
         <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E14" t="s">
         <v>137</v>
@@ -1648,18 +1637,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B15" t="s">
         <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E15" t="s">
         <v>36</v>
@@ -1682,28 +1671,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="6" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="6" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1714,23 +1703,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1740,11 +1729,11 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1754,17 +1743,17 @@
       <c r="C4" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1774,17 +1763,17 @@
       <c r="C5" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1794,17 +1783,17 @@
       <c r="C6" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1814,17 +1803,17 @@
       <c r="C7" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1834,13 +1823,13 @@
       <c r="C8" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1858,28 +1847,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
     <col min="4" max="4" width="58" customWidth="1"/>
-    <col min="5" max="6" width="27.42578125" customWidth="1"/>
+    <col min="5" max="6" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1890,23 +1879,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1916,11 +1905,11 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1930,17 +1919,17 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1950,17 +1939,17 @@
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1970,17 +1959,17 @@
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1990,17 +1979,17 @@
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -2010,17 +1999,17 @@
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -2030,17 +2019,17 @@
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2050,17 +2039,17 @@
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -2070,17 +2059,17 @@
       <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -2090,17 +2079,17 @@
       <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2110,17 +2099,17 @@
       <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2130,17 +2119,17 @@
       <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -2150,17 +2139,17 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -2170,17 +2159,17 @@
       <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -2190,17 +2179,17 @@
       <c r="C17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -2210,17 +2199,17 @@
       <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -2230,17 +2219,17 @@
       <c r="C19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -2250,17 +2239,17 @@
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -2270,17 +2259,17 @@
       <c r="C21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
@@ -2290,17 +2279,17 @@
       <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
@@ -2310,17 +2299,17 @@
       <c r="C23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
@@ -2330,17 +2319,17 @@
       <c r="C24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
@@ -2350,17 +2339,17 @@
       <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
@@ -2370,17 +2359,17 @@
       <c r="C26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
@@ -2390,17 +2379,17 @@
       <c r="C27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
@@ -2410,17 +2399,17 @@
       <c r="C28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
@@ -2430,17 +2419,17 @@
       <c r="C29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
@@ -2450,17 +2439,17 @@
       <c r="C30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
@@ -2470,17 +2459,17 @@
       <c r="C31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
@@ -2490,23 +2479,23 @@
       <c r="C32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2522,28 +2511,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="62.7109375" customWidth="1"/>
-    <col min="5" max="6" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" customWidth="1"/>
+    <col min="5" max="6" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2554,23 +2543,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -2580,471 +2569,471 @@
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="F8" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="F9" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="E12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="F13" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="F15" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="F16" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="F18" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="F19" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="F23" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="F24" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="F25" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -3057,14 +3046,14 @@
       <c r="D27" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="13">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -3077,14 +3066,14 @@
       <c r="D28" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3097,14 +3086,14 @@
       <c r="D29" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3117,14 +3106,14 @@
       <c r="D30" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="13">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -3137,14 +3126,14 @@
       <c r="D31" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -3157,14 +3146,14 @@
       <c r="D32" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -3177,14 +3166,14 @@
       <c r="D33" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -3197,14 +3186,14 @@
       <c r="D34" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="13">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -3217,10 +3206,10 @@
       <c r="D35" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="13">
         <v>35</v>
       </c>
     </row>
@@ -3238,55 +3227,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="62.7109375" style="13" customWidth="1"/>
-    <col min="5" max="6" width="27.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" style="12" customWidth="1"/>
+    <col min="5" max="6" width="27.5" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -3296,21 +3285,21 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -3320,17 +3309,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -3340,17 +3329,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -3360,17 +3349,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -3380,17 +3369,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -3400,17 +3389,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -3420,17 +3409,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -3440,17 +3429,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -3460,17 +3449,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -3480,17 +3469,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -3500,17 +3489,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -3520,17 +3509,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -3540,17 +3529,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -3560,17 +3549,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -3580,17 +3569,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -3600,17 +3589,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -3620,17 +3609,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -3640,17 +3629,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="3" t="s">
         <v>72</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -3660,17 +3649,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -3680,17 +3669,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -3700,17 +3689,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="3" t="s">
         <v>75</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -3720,17 +3709,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -3740,17 +3729,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -3760,17 +3749,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -3780,17 +3769,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -3800,17 +3789,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -3820,17 +3809,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -3840,17 +3829,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -3860,17 +3849,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -3880,17 +3869,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="3" t="s">
         <v>77</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -3900,17 +3889,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -3920,17 +3909,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -3940,17 +3929,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -3960,17 +3949,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -3980,17 +3969,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -4001,7 +3990,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D64">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D64">
     <sortCondition ref="B1"/>
   </sortState>
   <mergeCells count="5">
@@ -4017,55 +4006,55 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="62.7109375" style="13" customWidth="1"/>
-    <col min="5" max="6" width="27.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" style="12" customWidth="1"/>
+    <col min="5" max="6" width="27.5" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -4075,21 +4064,21 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -4099,17 +4088,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -4119,17 +4108,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -4139,17 +4128,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="3" t="s">
         <v>109</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -4159,17 +4148,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -4179,17 +4168,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -4199,17 +4188,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="3" t="s">
         <v>111</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -4219,17 +4208,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -4239,17 +4228,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -4259,17 +4248,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -4279,17 +4268,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -4299,17 +4288,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -4319,17 +4308,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -4339,17 +4328,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -4359,17 +4348,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -4379,17 +4368,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -4399,17 +4388,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -4419,17 +4408,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -4439,17 +4428,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -4459,17 +4448,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -4479,17 +4468,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -4499,17 +4488,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -4519,17 +4508,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="3" t="s">
         <v>102</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -4539,17 +4528,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -4559,17 +4548,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -4579,17 +4568,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="3" t="s">
         <v>115</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -4599,17 +4588,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -4619,17 +4608,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -4639,17 +4628,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -4659,17 +4648,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -4679,17 +4668,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="3" t="s">
         <v>117</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -4699,17 +4688,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -4719,17 +4708,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -4739,17 +4728,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="3" t="s">
         <v>118</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -4759,17 +4748,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="3" t="s">
         <v>75</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -4779,17 +4768,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="3" t="s">
         <v>119</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -4813,12 +4802,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>